<commit_message>
modified:   tutorial/supply/readme.md 	modified:   "tutorial/supply/tests/supplier_excel_data/\344\270\273\346\234\272\346\225\260\346\215\256\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/tutorial/supply/tests/supplier_excel_data/主机数据表.xlsx
+++ b/tutorial/supply/tests/supplier_excel_data/主机数据表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengzhenbo/Library/Mobile Documents/com~apple~CloudDocs/04Project/ElevatorCertificate/ElevatorCertificate/tutorial/supply/供应商数据表/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengzhenbo/Library/Mobile Documents/com~apple~CloudDocs/04Project/ElevatorCertificate/ElevatorCertificate/tutorial/supply/tests/supplier_excel_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20880FDB-1325-8947-B2C9-8C62F3529393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DCA78-11E2-0348-B942-2A30B24FC4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39020" yWindow="2280" windowWidth="28180" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7100" yWindow="520" windowWidth="24260" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="主机数据" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>合同号</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>2023.7.29</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品型号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>编号1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>编号2</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -750,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -879,13 +891,13 @@
         <v>20</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>15</v>

</xml_diff>